<commit_message>
Update to correct test case
</commit_message>
<xml_diff>
--- a/tests/financial_calculations.xlsx
+++ b/tests/financial_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\FinancialCalculations\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE14E6E-C7F0-475D-856E-57C6504DE4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CC6938-548B-4967-8C5D-8E3334C7FB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2FC359D8-ED62-4E60-AC8A-E682B0C526C5}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>future_value + 10</t>
   </si>
   <si>
-    <t>current * (1 + rate) ** year</t>
+    <t>current * (1 + rate) * year</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>